<commit_message>
Add reason to not complete on Visit ODK Form
</commit_message>
<xml_diff>
--- a/xforms/xlsforms/visit_registration.xlsx
+++ b/xforms/xlsforms/visit_registration.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="630" yWindow="510" windowWidth="15600" windowHeight="11760" tabRatio="500"/>
+    <workbookView xWindow="630" yWindow="510" windowWidth="15600" windowHeight="11640" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="166">
   <si>
     <t>type</t>
   </si>
@@ -267,9 +267,6 @@
     <t>concat(substr(${locationIdCheck},0,3),'0000',substr(${locationIdCheck},3,5))</t>
   </si>
   <si>
-    <t>../farmhouse = '1' and (${locationId} !=${locationcalculated})</t>
-  </si>
-  <si>
     <t>reasonnotin</t>
   </si>
   <si>
@@ -409,6 +406,114 @@
   </si>
   <si>
     <t>Registo de Visita</t>
+  </si>
+  <si>
+    <t>reason_to_not_complete</t>
+  </si>
+  <si>
+    <t>Casa não encontrada</t>
+  </si>
+  <si>
+    <t>Casa destruída</t>
+  </si>
+  <si>
+    <t>Casa desabitada</t>
+  </si>
+  <si>
+    <t>Sem informante</t>
+  </si>
+  <si>
+    <t>Outro motivo</t>
+  </si>
+  <si>
+    <t>Não sabe</t>
+  </si>
+  <si>
+    <t>Recusa.</t>
+  </si>
+  <si>
+    <t>select_one yes_no</t>
+  </si>
+  <si>
+    <t>completedQuest</t>
+  </si>
+  <si>
+    <t>Inquérito completo?</t>
+  </si>
+  <si>
+    <t>select_one reason_to_not_complete</t>
+  </si>
+  <si>
+    <t>reasonToNotComplete</t>
+  </si>
+  <si>
+    <t>Motivo de não ter completado o inquérito?</t>
+  </si>
+  <si>
+    <t>${completedQuest}=2</t>
+  </si>
+  <si>
+    <t>${completedQuest}!=2</t>
+  </si>
+  <si>
+    <t>select_one houseno_locations</t>
+  </si>
+  <si>
+    <t>houseNoLocated</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Localização do número do agregado?</t>
+  </si>
+  <si>
+    <t>houseNoNeedRepaint</t>
+  </si>
+  <si>
+    <t>A casa precisa ser repintada?</t>
+  </si>
+  <si>
+    <t>../farmhouse = '1' and (${locationId} !=${locationcalculated}) and ${completedQuest}!=2</t>
+  </si>
+  <si>
+    <t>Inquérito completo/A casa foi visitada?</t>
+  </si>
+  <si>
+    <t>Motivo de não ter completado o inquérito/visitado a casa?</t>
+  </si>
+  <si>
+    <t>O numero da casa precisa ser repintada?</t>
+  </si>
+  <si>
+    <t>yes_no</t>
+  </si>
+  <si>
+    <t>Não</t>
+  </si>
+  <si>
+    <t>houseno_locations</t>
+  </si>
+  <si>
+    <t>Porta</t>
+  </si>
+  <si>
+    <t>Parede</t>
+  </si>
+  <si>
+    <t>Árvore</t>
+  </si>
+  <si>
+    <t>Porta de quintal</t>
+  </si>
+  <si>
+    <t>Outro Local</t>
+  </si>
+  <si>
+    <t>reasonTncEspecified</t>
+  </si>
+  <si>
+    <t>Especifique o motivo de não ter completado o inquerito?</t>
+  </si>
+  <si>
+    <t>${completedQuest}=5</t>
   </si>
 </sst>
 </file>
@@ -484,7 +589,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="351">
+  <cellStyleXfs count="1051">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -836,8 +941,708 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -878,8 +1683,30 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="351">
+  <cellStyles count="1051">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1055,6 +1882,356 @@
     <cellStyle name="Followed Hyperlink" xfId="346" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="348" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="350" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="352" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="354" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="356" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="358" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="360" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="362" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="364" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="366" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="368" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="370" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="372" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="374" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="376" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="378" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="380" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="382" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="384" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="386" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="388" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="390" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="392" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="394" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="396" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="398" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="400" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="402" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="404" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="406" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="408" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="410" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="412" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="414" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="416" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="418" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="420" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="422" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="424" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="426" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="428" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="430" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="432" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="434" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="436" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="438" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="440" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="442" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="444" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="446" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="448" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="450" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="452" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="454" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="456" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="458" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="460" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="462" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="464" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="466" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="468" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="470" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="472" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="474" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="476" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="478" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="480" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="482" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="484" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="486" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="488" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="490" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="492" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="494" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="496" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="498" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="500" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="502" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="504" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="506" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="508" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="510" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="512" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="514" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="516" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="518" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="520" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="522" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="524" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="526" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="528" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="530" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="532" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="534" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="536" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="538" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="540" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="542" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="544" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="546" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="548" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="550" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="552" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="554" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="556" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="558" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="560" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="562" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="564" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="566" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="568" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="570" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="572" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="574" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="576" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="578" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="580" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="582" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="584" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="586" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="588" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="590" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="592" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="594" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="596" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="598" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="600" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="602" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="604" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="606" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="608" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="610" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="612" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="614" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="616" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="618" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="620" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="622" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="624" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="626" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="628" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="630" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="632" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="634" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="636" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="638" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="640" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="642" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="644" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="646" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="648" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="650" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="652" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="654" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="656" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="658" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="660" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="662" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="664" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="666" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="668" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="670" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="672" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="674" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="676" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="678" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="680" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="682" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="684" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="686" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="688" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="690" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="692" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="694" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="696" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="698" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="700" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="702" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="704" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="706" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="708" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="710" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="712" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="714" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="716" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="718" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="720" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="722" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="724" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="726" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="728" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="730" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="732" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="734" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="736" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="738" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="740" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="742" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="744" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="746" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="748" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="750" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="752" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="754" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="756" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="758" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="760" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="762" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="764" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="766" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="768" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="770" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="772" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="774" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="776" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="778" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="780" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="782" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="784" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="786" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="788" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="790" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="792" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="794" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="796" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="798" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="800" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="802" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="804" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="806" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="808" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="810" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="812" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="814" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="816" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="818" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="820" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="822" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="824" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="826" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="828" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="830" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="832" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="834" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="836" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="838" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="840" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="842" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="844" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="846" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="848" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="850" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="852" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="854" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="856" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="858" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="860" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="862" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="864" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="866" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="868" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="870" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="872" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="874" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="876" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="878" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="880" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="882" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="884" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="886" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="888" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="890" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="892" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="894" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="896" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="898" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="900" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="902" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="904" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="906" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="908" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="910" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="912" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="914" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="916" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="918" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="920" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="922" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="924" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="926" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="928" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="930" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="932" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="934" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="936" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="938" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="940" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="942" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="944" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="946" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="948" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="950" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="952" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="954" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="956" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="958" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="960" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="962" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="964" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="966" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="968" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="970" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="972" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="974" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="976" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="978" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="980" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="982" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="984" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="986" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="988" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="990" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="992" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="994" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="996" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="998" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1000" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1002" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1004" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1006" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1008" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1010" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1012" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1014" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1016" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1018" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1020" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1022" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1024" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1026" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1028" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1030" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1032" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1034" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1036" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1038" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1040" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1042" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1044" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1046" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1048" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1050" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1230,15 +2407,360 @@
     <cellStyle name="Hyperlink" xfId="345" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="347" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="349" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="351" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="353" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="355" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="357" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="359" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="361" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="363" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="365" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="367" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="369" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="371" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="373" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="375" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="377" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="379" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="381" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="383" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="385" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="387" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="389" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="391" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="393" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="395" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="397" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="399" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="401" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="403" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="405" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="407" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="409" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="411" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="413" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="415" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="417" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="419" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="421" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="423" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="425" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="427" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="429" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="431" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="433" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="435" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="437" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="439" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="441" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="443" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="445" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="447" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="449" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="451" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="453" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="455" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="457" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="459" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="461" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="463" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="465" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="467" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="469" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="471" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="473" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="475" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="477" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="479" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="481" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="483" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="485" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="487" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="489" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="491" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="493" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="495" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="497" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="499" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="501" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="503" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="505" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="507" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="509" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="511" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="513" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="515" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="517" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="519" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="521" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="523" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="525" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="527" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="529" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="531" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="533" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="535" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="537" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="539" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="541" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="543" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="545" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="547" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="549" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="551" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="553" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="555" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="557" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="559" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="561" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="563" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="565" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="567" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="569" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="571" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="573" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="575" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="577" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="579" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="581" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="583" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="585" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="587" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="589" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="591" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="593" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="595" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="597" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="599" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="601" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="603" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="605" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="607" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="609" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="611" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="613" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="615" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="617" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="619" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="621" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="623" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="625" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="627" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="629" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="631" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="633" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="635" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="637" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="639" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="641" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="643" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="645" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="647" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="649" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="651" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="653" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="655" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="657" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="659" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="661" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="663" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="665" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="667" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="669" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="671" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="673" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="675" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="677" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="679" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="681" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="683" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="685" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="687" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="689" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="691" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="693" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="695" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="697" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="699" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="701" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="703" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="705" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="707" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="709" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="711" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="713" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="715" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="717" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="719" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="721" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="723" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="725" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="727" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="729" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="731" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="733" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="735" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="737" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="739" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="741" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="743" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="745" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="747" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="749" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="751" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="753" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="755" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="757" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="759" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="761" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="763" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="765" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="767" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="769" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="771" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="773" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="775" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="777" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="779" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="781" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="783" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="785" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="787" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="789" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="791" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="793" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="795" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="797" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="799" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="801" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="803" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="805" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="807" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="809" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="811" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="813" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="815" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="817" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="819" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="821" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="823" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="825" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="827" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="829" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="831" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="833" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="835" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="837" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="839" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="841" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="843" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="845" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="847" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="849" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="851" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="853" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="855" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="857" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="859" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="861" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="863" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="865" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="867" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="869" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="871" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="873" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="875" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="877" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="879" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="881" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="883" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="885" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="887" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="889" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="891" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="893" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="895" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="897" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="899" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="901" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="903" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="905" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="907" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="909" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="911" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="913" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="915" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="917" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="919" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="921" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="923" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="925" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="927" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="929" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="931" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="933" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="935" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="937" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="939" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="941" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="943" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="945" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="947" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="949" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="951" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="953" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="955" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="957" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="959" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="961" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="963" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="965" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="967" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="969" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="971" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="973" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="975" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="977" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="979" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="981" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="983" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="985" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="987" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="989" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="991" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="993" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="995" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="997" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="999" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1001" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1003" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1005" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1007" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1009" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1011" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1013" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1015" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1017" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1019" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1021" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1023" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1025" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1027" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1029" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1031" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1033" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1035" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1037" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1039" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1041" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1043" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1045" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1047" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1049" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -1564,20 +3086,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R89"/>
+  <dimension ref="A1:R94"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="101" zoomScaleNormal="101" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="101" zoomScaleNormal="101" zoomScalePageLayoutView="125" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="H14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J20" sqref="J20"/>
+      <selection pane="bottomRight" activeCell="A21" sqref="A21:XFD21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12"/>
+  <sheetFormatPr defaultRowHeight="12"/>
   <cols>
     <col min="1" max="1" width="23.375" style="5" customWidth="1"/>
     <col min="2" max="2" width="18.5" style="5" customWidth="1"/>
-    <col min="3" max="3" width="39.625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="43.875" style="5" customWidth="1"/>
     <col min="4" max="4" width="35.375" style="5" customWidth="1"/>
     <col min="5" max="5" width="29.875" style="5" customWidth="1"/>
     <col min="6" max="6" width="18" style="5" customWidth="1"/>
@@ -1587,10 +3109,10 @@
     <col min="10" max="11" width="10.875" style="5"/>
     <col min="12" max="12" width="19.125" style="5" customWidth="1"/>
     <col min="13" max="13" width="34.125" style="5" customWidth="1"/>
-    <col min="14" max="16384" width="10.875" style="5"/>
+    <col min="14" max="16384" width="9" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:18" ht="24">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1598,7 +3120,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>18</v>
@@ -1717,7 +3239,7 @@
         <v>22</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>23</v>
@@ -1749,7 +3271,7 @@
         <v>24</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>25</v>
@@ -1772,7 +3294,7 @@
         <v>26</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>27</v>
@@ -1792,16 +3314,16 @@
         <v>21</v>
       </c>
       <c r="B8" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="D8" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="D8" s="5" t="s">
+      <c r="E8" s="5" t="s">
         <v>102</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>103</v>
       </c>
       <c r="J8" s="4" t="b">
         <v>1</v>
@@ -1812,19 +3334,19 @@
     </row>
     <row r="9" spans="1:18" ht="15" customHeight="1">
       <c r="A9" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="C9" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="C9" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>92</v>
-      </c>
       <c r="E9" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J9" s="4" t="b">
         <v>1</v>
@@ -1841,7 +3363,7 @@
         <v>68</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>27</v>
@@ -1851,7 +3373,7 @@
       </c>
       <c r="J10" s="4"/>
       <c r="M10" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="N10" s="4"/>
     </row>
@@ -1863,7 +3385,7 @@
         <v>80</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>81</v>
@@ -1876,7 +3398,7 @@
         <v>82</v>
       </c>
       <c r="M11" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="N11" s="4" t="b">
         <v>1</v>
@@ -1890,7 +3412,7 @@
         <v>69</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>71</v>
@@ -1899,7 +3421,7 @@
         <v>1</v>
       </c>
       <c r="M12" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="N12" s="4"/>
     </row>
@@ -1911,7 +3433,7 @@
         <v>72</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>73</v>
@@ -1920,7 +3442,7 @@
         <v>1</v>
       </c>
       <c r="M13" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="N13" s="4"/>
     </row>
@@ -1932,7 +3454,7 @@
         <v>29</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>30</v>
@@ -1955,7 +3477,7 @@
         <v>31</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>25</v>
@@ -1978,7 +3500,7 @@
         <v>33</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>34</v>
@@ -1998,7 +3520,7 @@
         <v>35</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>36</v>
@@ -2015,13 +3537,13 @@
     </row>
     <row r="18" spans="1:14">
       <c r="A18" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>38</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>37</v>
@@ -2036,136 +3558,240 @@
         <v>62</v>
       </c>
     </row>
-    <row r="19" spans="1:14">
-      <c r="A19" s="10" t="s">
+    <row r="19" spans="1:14" s="16" customFormat="1" ht="15">
+      <c r="A19" s="20" t="s">
+        <v>138</v>
+      </c>
+      <c r="B19" s="20" t="s">
+        <v>139</v>
+      </c>
+      <c r="C19" s="20" t="s">
+        <v>152</v>
+      </c>
+      <c r="D19" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="E19" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="F19" s="17"/>
+      <c r="G19" s="17"/>
+      <c r="H19" s="17"/>
+      <c r="I19" s="17"/>
+      <c r="J19" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="K19" s="17"/>
+      <c r="L19" s="17"/>
+      <c r="M19" s="17"/>
+      <c r="N19" s="17"/>
+    </row>
+    <row r="20" spans="1:14" s="16" customFormat="1" ht="24.75">
+      <c r="A20" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="B20" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="C20" s="20" t="s">
+        <v>153</v>
+      </c>
+      <c r="D20" s="20" t="s">
+        <v>143</v>
+      </c>
+      <c r="E20" s="20" t="s">
+        <v>143</v>
+      </c>
+      <c r="F20" s="17"/>
+      <c r="G20" s="17"/>
+      <c r="H20" s="17"/>
+      <c r="I20" s="17"/>
+      <c r="J20" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="K20" s="17"/>
+      <c r="L20" s="17"/>
+      <c r="M20" s="20" t="s">
+        <v>144</v>
+      </c>
+      <c r="N20" s="17"/>
+    </row>
+    <row r="21" spans="1:14" s="20" customFormat="1" ht="24.75">
+      <c r="A21" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" s="20" t="s">
+        <v>163</v>
+      </c>
+      <c r="C21" s="20" t="s">
+        <v>164</v>
+      </c>
+      <c r="D21" s="20" t="s">
+        <v>164</v>
+      </c>
+      <c r="E21" s="20" t="s">
+        <v>164</v>
+      </c>
+      <c r="F21" s="17"/>
+      <c r="G21" s="17"/>
+      <c r="H21" s="17"/>
+      <c r="I21" s="17"/>
+      <c r="J21" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="K21" s="17"/>
+      <c r="L21" s="17"/>
+      <c r="M21" s="20" t="s">
+        <v>165</v>
+      </c>
+      <c r="N21" s="17"/>
+    </row>
+    <row r="22" spans="1:14" s="16" customFormat="1" ht="15">
+      <c r="A22" s="23" t="s">
+        <v>146</v>
+      </c>
+      <c r="B22" s="23" t="s">
+        <v>147</v>
+      </c>
+      <c r="C22" s="22" t="s">
+        <v>148</v>
+      </c>
+      <c r="D22" s="22" t="s">
+        <v>148</v>
+      </c>
+      <c r="E22" s="22" t="s">
+        <v>148</v>
+      </c>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
+      <c r="H22" s="18"/>
+      <c r="I22" s="17"/>
+      <c r="J22" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="K22" s="17"/>
+      <c r="L22" s="17"/>
+      <c r="M22" s="20" t="s">
+        <v>145</v>
+      </c>
+      <c r="N22" s="17"/>
+    </row>
+    <row r="23" spans="1:14" ht="15">
+      <c r="A23" s="23" t="s">
+        <v>138</v>
+      </c>
+      <c r="B23" s="23" t="s">
+        <v>149</v>
+      </c>
+      <c r="C23" s="22" t="s">
+        <v>154</v>
+      </c>
+      <c r="D23" s="22" t="s">
+        <v>150</v>
+      </c>
+      <c r="E23" s="22" t="s">
+        <v>150</v>
+      </c>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="18"/>
+      <c r="I23" s="17"/>
+      <c r="J23" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="K23" s="17"/>
+      <c r="L23" s="17"/>
+      <c r="M23" s="20" t="s">
+        <v>145</v>
+      </c>
+      <c r="N23" s="17"/>
+    </row>
+    <row r="24" spans="1:14" s="16" customFormat="1" ht="15">
+      <c r="A24" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="B19" s="10" t="s">
+      <c r="B24" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="C19" s="9" t="s">
+      <c r="C24" s="22" t="s">
+        <v>113</v>
+      </c>
+      <c r="D24" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="E24" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
+      <c r="H24" s="18"/>
+      <c r="I24" s="17"/>
+      <c r="J24" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="K24" s="17"/>
+      <c r="L24" s="17"/>
+      <c r="M24" s="20" t="s">
+        <v>145</v>
+      </c>
+      <c r="N24" s="17"/>
+    </row>
+    <row r="25" spans="1:14" ht="39.75" customHeight="1">
+      <c r="A25" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C25" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="D19" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E19" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-      <c r="J19" s="4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" ht="24">
-      <c r="A20" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="B20" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="C20" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="D20" s="2" t="s">
+      <c r="D25" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E20" s="9" t="s">
+      <c r="E25" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-      <c r="J20" s="4"/>
-      <c r="M20" s="5" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14">
-      <c r="A21" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="E21" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="N21" s="4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14">
-      <c r="A22" s="7"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-    </row>
-    <row r="23" spans="1:14">
-      <c r="A23" s="7"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="11"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
-    </row>
-    <row r="24" spans="1:14">
-      <c r="A24" s="2"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-    </row>
-    <row r="25" spans="1:14">
-      <c r="A25" s="2"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
+      <c r="J25" s="4"/>
+      <c r="M25" s="20" t="s">
+        <v>151</v>
+      </c>
     </row>
     <row r="26" spans="1:14">
-      <c r="A26" s="2"/>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
-      <c r="J26" s="3"/>
+      <c r="A26" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="N26" s="4" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="27" spans="1:14">
-      <c r="A27" s="2"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="11"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="11"/>
+      <c r="A27" s="7"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="2"/>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
     </row>
     <row r="28" spans="1:14">
-      <c r="A28" s="2"/>
+      <c r="A28" s="7"/>
       <c r="B28" s="2"/>
       <c r="C28" s="11"/>
       <c r="D28" s="2"/>
@@ -2203,13 +3829,14 @@
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
+      <c r="J31" s="3"/>
     </row>
     <row r="32" spans="1:14">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
+      <c r="C32" s="11"/>
       <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
+      <c r="E32" s="11"/>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
@@ -2217,13 +3844,12 @@
     <row r="33" spans="1:10">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
+      <c r="C33" s="11"/>
       <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
+      <c r="E33" s="11"/>
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
-      <c r="J33" s="3"/>
     </row>
     <row r="34" spans="1:10">
       <c r="A34" s="2"/>
@@ -2234,7 +3860,6 @@
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
-      <c r="J34" s="3"/>
     </row>
     <row r="35" spans="1:10">
       <c r="A35" s="2"/>
@@ -2245,7 +3870,6 @@
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
-      <c r="J35" s="3"/>
     </row>
     <row r="36" spans="1:10">
       <c r="A36" s="2"/>
@@ -2266,64 +3890,117 @@
       <c r="F37" s="2"/>
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
-      <c r="J37" s="3"/>
+    </row>
+    <row r="38" spans="1:10">
+      <c r="A38" s="2"/>
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
+      <c r="J38" s="3"/>
+    </row>
+    <row r="39" spans="1:10">
+      <c r="A39" s="2"/>
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
+      <c r="J39" s="3"/>
+    </row>
+    <row r="40" spans="1:10">
+      <c r="A40" s="2"/>
+      <c r="B40" s="2"/>
+      <c r="C40" s="2"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+      <c r="G40" s="2"/>
+      <c r="H40" s="2"/>
+      <c r="J40" s="3"/>
     </row>
     <row r="41" spans="1:10">
-      <c r="J41" s="3"/>
+      <c r="A41" s="2"/>
+      <c r="B41" s="2"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+      <c r="F41" s="2"/>
+      <c r="G41" s="2"/>
+      <c r="H41" s="2"/>
     </row>
     <row r="42" spans="1:10">
+      <c r="A42" s="2"/>
+      <c r="B42" s="2"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
+      <c r="F42" s="2"/>
+      <c r="G42" s="2"/>
+      <c r="H42" s="2"/>
       <c r="J42" s="3"/>
     </row>
-    <row r="50" spans="10:10">
-      <c r="J50" s="3"/>
-    </row>
-    <row r="58" spans="10:10">
-      <c r="J58" s="3"/>
-    </row>
-    <row r="59" spans="10:10">
-      <c r="J59" s="3"/>
-    </row>
-    <row r="60" spans="10:10">
-      <c r="J60" s="3"/>
-    </row>
-    <row r="61" spans="10:10">
-      <c r="J61" s="3"/>
-    </row>
-    <row r="62" spans="10:10">
-      <c r="J62" s="3"/>
-    </row>
-    <row r="79" spans="10:10">
-      <c r="J79" s="3"/>
-    </row>
-    <row r="80" spans="10:10">
-      <c r="J80" s="3"/>
-    </row>
-    <row r="81" spans="1:10">
-      <c r="J81" s="3"/>
-    </row>
-    <row r="82" spans="1:10">
-      <c r="J82" s="3"/>
-    </row>
-    <row r="83" spans="1:10">
-      <c r="J83" s="3"/>
+    <row r="46" spans="1:10">
+      <c r="J46" s="3"/>
+    </row>
+    <row r="47" spans="1:10">
+      <c r="J47" s="3"/>
+    </row>
+    <row r="55" spans="10:10">
+      <c r="J55" s="3"/>
+    </row>
+    <row r="63" spans="10:10">
+      <c r="J63" s="3"/>
+    </row>
+    <row r="64" spans="10:10">
+      <c r="J64" s="3"/>
+    </row>
+    <row r="65" spans="10:10">
+      <c r="J65" s="3"/>
+    </row>
+    <row r="66" spans="10:10">
+      <c r="J66" s="3"/>
+    </row>
+    <row r="67" spans="10:10">
+      <c r="J67" s="3"/>
     </row>
     <row r="84" spans="1:10">
-      <c r="A84" s="3"/>
       <c r="J84" s="3"/>
     </row>
     <row r="85" spans="1:10">
-      <c r="A85" s="3"/>
       <c r="J85" s="3"/>
     </row>
     <row r="86" spans="1:10">
-      <c r="A86" s="3"/>
       <c r="J86" s="3"/>
     </row>
     <row r="87" spans="1:10">
       <c r="J87" s="3"/>
     </row>
+    <row r="88" spans="1:10">
+      <c r="J88" s="3"/>
+    </row>
     <row r="89" spans="1:10">
+      <c r="A89" s="3"/>
       <c r="J89" s="3"/>
+    </row>
+    <row r="90" spans="1:10">
+      <c r="A90" s="3"/>
+      <c r="J90" s="3"/>
+    </row>
+    <row r="91" spans="1:10">
+      <c r="A91" s="3"/>
+      <c r="J91" s="3"/>
+    </row>
+    <row r="92" spans="1:10">
+      <c r="J92" s="3"/>
+    </row>
+    <row r="94" spans="1:10">
+      <c r="J94" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2333,15 +4010,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E68"/>
+  <dimension ref="A1:E70"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18:E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12"/>
   <cols>
-    <col min="1" max="1" width="13.75" style="5" customWidth="1"/>
+    <col min="1" max="1" width="20.25" style="5" customWidth="1"/>
     <col min="2" max="2" width="13" style="5" customWidth="1"/>
     <col min="3" max="3" width="22.25" style="5" customWidth="1"/>
     <col min="4" max="4" width="19.5" style="5" customWidth="1"/>
@@ -2357,7 +4034,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>18</v>
@@ -2366,259 +4043,413 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="13">
-        <v>0</v>
-      </c>
-      <c r="C2" s="14" t="s">
+    <row r="2" spans="1:5" s="20" customFormat="1">
+      <c r="A2" s="19" t="s">
+        <v>155</v>
+      </c>
+      <c r="B2" s="25">
+        <v>1</v>
+      </c>
+      <c r="C2" s="21" t="s">
         <v>118</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2" s="21" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="20" customFormat="1">
+      <c r="A3" s="19" t="s">
+        <v>155</v>
+      </c>
+      <c r="B3" s="25">
+        <v>2</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>156</v>
+      </c>
+      <c r="D3" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E3" s="21" t="s">
         <v>47</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="B3" s="13">
-        <v>1</v>
-      </c>
-      <c r="C3" s="14" t="s">
-        <v>119</v>
-      </c>
-      <c r="D3" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="E3" s="14" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="12" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="B4" s="13">
         <v>0</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>74</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="12" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="B5" s="13">
         <v>1</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="12" t="s">
-        <v>79</v>
+        <v>40</v>
       </c>
       <c r="B6" s="13">
         <v>0</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>75</v>
+        <v>49</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="12" t="s">
-        <v>79</v>
+        <v>40</v>
       </c>
       <c r="B7" s="13">
         <v>1</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>77</v>
+        <v>50</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>77</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="12" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B8" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="B9" s="13">
+        <v>1</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="B10" s="13">
+        <v>1</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="D10" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="B9" s="13">
+      <c r="E10" s="14" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="B11" s="13">
         <v>2</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="C11" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="15">
+      <c r="A12" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="B12" s="13">
+        <v>3</v>
+      </c>
+      <c r="C12" s="14" t="s">
         <v>125</v>
       </c>
-      <c r="D9" s="14" t="s">
-        <v>86</v>
-      </c>
-      <c r="E9" s="14" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="15">
-      <c r="A10" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="B10" s="13">
+      <c r="D12" t="s">
+        <v>87</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="15">
+      <c r="A13" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="B13" s="13">
+        <v>99</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="D13" t="s">
+        <v>88</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="B14" s="13">
+        <v>1</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="B15" s="13">
+        <v>2</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="B16" s="13">
         <v>3</v>
       </c>
-      <c r="C10" s="14" t="s">
-        <v>126</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="C16" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="B17" s="13">
+        <v>4</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="B18" s="13">
+        <v>5</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="B19" s="13">
         <v>88</v>
       </c>
-      <c r="E10" s="14" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="15">
-      <c r="A11" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="B11" s="13">
+      <c r="C19" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="B20" s="13">
         <v>99</v>
       </c>
-      <c r="C11" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="D11" t="s">
-        <v>89</v>
-      </c>
-      <c r="E11" s="14" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="12"/>
-      <c r="B12" s="13"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="12"/>
-      <c r="B13" s="13"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="12"/>
-      <c r="B14" s="13"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="12"/>
-      <c r="B15" s="13"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="12"/>
-      <c r="B16" s="13"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="12"/>
-      <c r="B17" s="13"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18" s="12"/>
-      <c r="B18" s="13"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" s="12"/>
-      <c r="B19" s="13"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="12"/>
-      <c r="B20" s="13"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
+      <c r="C20" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="12"/>
-      <c r="B21" s="13"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
+      <c r="A21" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="B21" s="13">
+        <v>1</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="E21" s="14" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22" s="12"/>
-      <c r="B22" s="13"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
+      <c r="A22" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="B22" s="13">
+        <v>2</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="D22" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="E22" s="14" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" s="12"/>
-      <c r="B23" s="13"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="14"/>
+      <c r="A23" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="B23" s="13">
+        <v>3</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="E23" s="14" t="s">
+        <v>160</v>
+      </c>
     </row>
     <row r="24" spans="1:5">
-      <c r="A24" s="12"/>
-      <c r="B24" s="13"/>
-      <c r="D24" s="14"/>
-      <c r="E24" s="14"/>
+      <c r="A24" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="B24" s="13">
+        <v>4</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="D24" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="E24" s="14" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="25" spans="1:5">
-      <c r="A25" s="12"/>
-      <c r="B25" s="13"/>
-      <c r="D25" s="14"/>
-      <c r="E25" s="14"/>
+      <c r="A25" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="B25" s="13">
+        <v>5</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="D25" s="14" t="s">
+        <v>162</v>
+      </c>
+      <c r="E25" s="14" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="12"/>
@@ -2722,19 +4553,19 @@
       <c r="D42" s="14"/>
       <c r="E42" s="14"/>
     </row>
-    <row r="43" spans="1:5" s="15" customFormat="1">
+    <row r="43" spans="1:5">
+      <c r="A43" s="12"/>
       <c r="B43" s="13"/>
       <c r="D43" s="14"/>
       <c r="E43" s="14"/>
     </row>
     <row r="44" spans="1:5">
-      <c r="A44" s="15"/>
+      <c r="A44" s="12"/>
       <c r="B44" s="13"/>
       <c r="D44" s="14"/>
       <c r="E44" s="14"/>
     </row>
-    <row r="45" spans="1:5">
-      <c r="A45" s="15"/>
+    <row r="45" spans="1:5" s="15" customFormat="1">
       <c r="B45" s="13"/>
       <c r="D45" s="14"/>
       <c r="E45" s="14"/>
@@ -2876,6 +4707,18 @@
       <c r="B68" s="13"/>
       <c r="D68" s="14"/>
       <c r="E68" s="14"/>
+    </row>
+    <row r="69" spans="1:5">
+      <c r="A69" s="15"/>
+      <c r="B69" s="13"/>
+      <c r="D69" s="14"/>
+      <c r="E69" s="14"/>
+    </row>
+    <row r="70" spans="1:5">
+      <c r="A70" s="15"/>
+      <c r="B70" s="13"/>
+      <c r="D70" s="14"/>
+      <c r="E70" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2910,21 +4753,21 @@
         <v>65</v>
       </c>
       <c r="D1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B2" t="s">
         <v>66</v>
       </c>
       <c r="C2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Creating exclusive task/button to synchronize pregnancies ids
</commit_message>
<xml_diff>
--- a/xforms/xlsforms/visit_registration.xlsx
+++ b/xforms/xlsforms/visit_registration.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="630" yWindow="510" windowWidth="15600" windowHeight="11640" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="630" yWindow="510" windowWidth="15600" windowHeight="11640" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -513,7 +513,7 @@
     <t>Especifique o motivo de não ter completado o inquerito?</t>
   </si>
   <si>
-    <t>${completedQuest}=5</t>
+    <t>${reasonToNotComplete}=5</t>
   </si>
 </sst>
 </file>
@@ -572,12 +572,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1642,7 +1648,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1704,6 +1710,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1051">
@@ -3088,11 +3097,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:R94"/>
   <sheetViews>
-    <sheetView zoomScale="101" zoomScaleNormal="101" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="H14" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="101" zoomScaleNormal="101" zoomScalePageLayoutView="125" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="I14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A21" sqref="A21:XFD21"/>
+      <selection pane="bottomRight" activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
@@ -3641,7 +3650,7 @@
       </c>
       <c r="K21" s="17"/>
       <c r="L21" s="17"/>
-      <c r="M21" s="20" t="s">
+      <c r="M21" s="26" t="s">
         <v>165</v>
       </c>
       <c r="N21" s="17"/>
@@ -4012,8 +4021,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:E18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14:C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12"/>

</xml_diff>